<commit_message>
add reconstruction example of cabinet
</commit_message>
<xml_diff>
--- a/建模进度/建模进度.xlsx
+++ b/建模进度/建模进度.xlsx
@@ -67,8 +67,8 @@
   <numFmts count="4">
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -88,21 +88,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -132,6 +118,43 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -185,46 +208,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,19 +263,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -293,157 +371,79 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,6 +454,32 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -468,6 +494,39 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -495,65 +554,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -562,10 +562,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -574,133 +574,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1071,7 +1071,7 @@
   <dimension ref="A2:P52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1122,6 +1122,7 @@
       <c r="D3" s="1"/>
       <c r="H3" s="1"/>
       <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
       <c r="O3" s="2"/>
       <c r="P3" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
update progress - liuyun_20211107
</commit_message>
<xml_diff>
--- a/建模进度/建模进度.xlsx
+++ b/建模进度/建模进度.xlsx
@@ -65,10 +65,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -88,12 +88,60 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -101,8 +149,23 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -116,15 +179,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -132,61 +209,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -200,31 +223,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -263,187 +263,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -457,13 +457,32 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -483,41 +502,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -526,7 +515,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -548,9 +537,20 @@
     <border>
       <left/>
       <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -562,10 +562,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -574,133 +574,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1070,8 +1070,8 @@
   <sheetPr/>
   <dimension ref="A2:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1185,7 +1185,7 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="C11" s="1"/>
+      <c r="C11" s="2"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:1">
@@ -1232,6 +1232,7 @@
       <c r="A19">
         <v>17</v>
       </c>
+      <c r="C19" s="2"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:1">
@@ -1344,7 +1345,7 @@
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="C38" s="1"/>
+      <c r="C38" s="2"/>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
@@ -1355,19 +1356,19 @@
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="C40" s="1"/>
+      <c r="C40" s="2"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="C41" s="1"/>
+      <c r="C41" s="2"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="C42" s="1"/>
+      <c r="C42" s="2"/>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">

</xml_diff>

<commit_message>
update progress - liuyun_20211108
</commit_message>
<xml_diff>
--- a/建模进度/建模进度.xlsx
+++ b/建模进度/建模进度.xlsx
@@ -65,10 +65,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -88,46 +88,88 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -142,89 +184,47 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -245,61 +245,151 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -311,139 +401,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -454,6 +454,30 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -468,6 +492,30 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -487,50 +535,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -545,15 +554,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -562,10 +562,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -574,133 +574,133 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="24" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="26" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1070,8 +1070,8 @@
   <sheetPr/>
   <dimension ref="A2:P52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -1120,10 +1120,11 @@
         <v>1</v>
       </c>
       <c r="D3" s="1"/>
-      <c r="H3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="H3" s="2"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
-      <c r="O3" s="2"/>
+      <c r="O3" s="3"/>
       <c r="P3" t="s">
         <v>11</v>
       </c>
@@ -1133,8 +1134,9 @@
         <v>2</v>
       </c>
       <c r="D4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="O4" s="3"/>
+      <c r="E4" s="1"/>
+      <c r="H4" s="2"/>
+      <c r="O4" s="2"/>
       <c r="P4" t="s">
         <v>12</v>
       </c>
@@ -1144,31 +1146,35 @@
         <v>3</v>
       </c>
       <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
       <c r="O5" s="4"/>
       <c r="P5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:5">
       <c r="A6">
         <v>4</v>
       </c>
       <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
         <v>5</v>
       </c>
       <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
     </row>
-    <row r="8" spans="1:4">
+    <row r="8" spans="1:5">
       <c r="A8">
         <v>6</v>
       </c>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
+      <c r="E8" s="3"/>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
@@ -1185,7 +1191,7 @@
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="C11" s="2"/>
+      <c r="C11" s="3"/>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:1">
@@ -1232,7 +1238,7 @@
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="C19" s="2"/>
+      <c r="C19" s="3"/>
       <c r="D19" s="1"/>
     </row>
     <row r="20" spans="1:1">
@@ -1294,7 +1300,7 @@
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="C29" s="2"/>
+      <c r="C29" s="3"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
@@ -1345,7 +1351,7 @@
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="C38" s="2"/>
+      <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:1">
       <c r="A39">
@@ -1356,19 +1362,19 @@
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="C40" s="2"/>
+      <c r="C40" s="3"/>
     </row>
     <row r="41" spans="1:3">
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="C41" s="2"/>
+      <c r="C41" s="3"/>
     </row>
     <row r="42" spans="1:3">
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="C42" s="2"/>
+      <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:2">
       <c r="A43">
@@ -1416,17 +1422,19 @@
       <c r="A50">
         <v>48</v>
       </c>
-      <c r="G50" s="1"/>
-    </row>
-    <row r="51" spans="1:1">
+      <c r="G50" s="4"/>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51">
         <v>49</v>
       </c>
-    </row>
-    <row r="52" spans="1:1">
+      <c r="G51" s="1"/>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52">
         <v>50</v>
       </c>
+      <c r="G52" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>